<commit_message>
Final results and activations visualization
</commit_message>
<xml_diff>
--- a/images/models.xlsx
+++ b/images/models.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="500" windowWidth="18480" windowHeight="14080" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
   <si>
     <t>LeNet</t>
   </si>
@@ -392,7 +392,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -432,8 +432,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -460,6 +462,42 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -469,44 +507,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -526,6 +537,7 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -545,6 +557,7 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -874,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F21"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -942,32 +955,38 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="24"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
+      <c r="A5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
@@ -982,213 +1001,186 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>11</v>
-      </c>
+      <c r="A7" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="24"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="10" t="s">
-        <v>5</v>
-      </c>
+      <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
+      <c r="D9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="13"/>
-      <c r="B10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="A10" s="10"/>
+      <c r="B10" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="24"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
       <c r="D11" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>12</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="13"/>
-      <c r="B12" s="11" t="s">
-        <v>4</v>
-      </c>
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
+      <c r="D12" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="E12" s="11"/>
       <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="13"/>
-      <c r="B13" s="11" t="s">
-        <v>5</v>
-      </c>
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
+      <c r="D13" s="13" t="s">
+        <v>4</v>
+      </c>
       <c r="E13" s="11"/>
       <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
+      <c r="A14" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
+      <c r="A15" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="27"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
+      <c r="A16" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="17"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="16" t="s">
+      <c r="A17" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="17"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>24</v>
+      <c r="A18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F19" s="20"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="21" t="s">
+      <c r="A19" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="23" t="s">
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="23"/>
-      <c r="F21" s="24"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
+  <mergeCells count="7">
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:F19"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A17:E17"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>